<commit_message>
right aligned column headers
</commit_message>
<xml_diff>
--- a/Tools/ElectrodeNamesKey/channel_listing.xlsx
+++ b/Tools/ElectrodeNamesKey/channel_listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesswift/Documents/git/VERA/Tools/ElectrodeNamesKey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2078F217-A8CB-8E4D-9E92-4D03421BC5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5258D635-E5B6-0A4A-BE21-F02DEEC45DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8140" yWindow="1800" windowWidth="33740" windowHeight="24060" xr2:uid="{25006F41-8D29-F34D-A29E-0682A80C5BBB}"/>
   </bookViews>
@@ -149,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -185,13 +185,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -216,6 +209,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +533,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,22 +550,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
       <c r="I1" s="2"/>
       <c r="J1" s="1"/>
     </row>
@@ -580,9 +577,9 @@
       <c r="D2" s="10">
         <v>1</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="26"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="23"/>
       <c r="H2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -593,9 +590,9 @@
       <c r="D3" s="5">
         <v>2</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="26"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="23"/>
       <c r="H3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -606,9 +603,9 @@
       <c r="D4" s="10">
         <v>3</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="26"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="23"/>
       <c r="H4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -619,9 +616,9 @@
       <c r="D5" s="5">
         <v>4</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="26"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="23"/>
       <c r="H5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -631,9 +628,9 @@
       <c r="D6" s="10">
         <v>5</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="26"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="23"/>
       <c r="H6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -643,9 +640,9 @@
       <c r="D7" s="5">
         <v>6</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="26"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="23"/>
       <c r="H7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -656,9 +653,9 @@
       <c r="D8" s="10">
         <v>7</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="26"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="23"/>
       <c r="H8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -669,9 +666,9 @@
       <c r="D9" s="5">
         <v>8</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="26"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="23"/>
       <c r="H9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -682,9 +679,9 @@
       <c r="D10" s="10">
         <v>9</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="26"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="23"/>
       <c r="H10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -695,9 +692,9 @@
       <c r="D11" s="5">
         <v>10</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="26"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="23"/>
       <c r="H11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -708,9 +705,9 @@
       <c r="D12" s="10">
         <v>11</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="26"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="23"/>
       <c r="H12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -721,9 +718,9 @@
       <c r="D13" s="5">
         <v>12</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="26"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="23"/>
       <c r="H13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -734,9 +731,9 @@
       <c r="D14" s="10">
         <v>13</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="26"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="23"/>
       <c r="H14"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -747,35 +744,35 @@
       <c r="D15" s="5">
         <v>14</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="26"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="23"/>
       <c r="H15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="20"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="10">
         <v>15</v>
       </c>
       <c r="D16" s="10">
         <v>15</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="26"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="23"/>
       <c r="H16"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="22"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="5">
         <v>16</v>
       </c>
       <c r="D17" s="5">
         <v>16</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="26"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="23"/>
       <c r="H17"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
@@ -786,9 +783,9 @@
       <c r="D18" s="10">
         <v>17</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="26"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="23"/>
       <c r="H18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
@@ -799,9 +796,9 @@
       <c r="D19" s="5">
         <v>18</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="26"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="23"/>
       <c r="H19"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
@@ -812,9 +809,9 @@
       <c r="D20" s="10">
         <v>19</v>
       </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="26"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="23"/>
       <c r="H20"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
@@ -825,9 +822,9 @@
       <c r="D21" s="5">
         <v>20</v>
       </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="26"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="23"/>
       <c r="H21"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
@@ -838,9 +835,9 @@
       <c r="D22" s="10">
         <v>21</v>
       </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="26"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="23"/>
       <c r="H22"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
@@ -851,9 +848,9 @@
       <c r="D23" s="5">
         <v>22</v>
       </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="26"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="23"/>
       <c r="H23"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
@@ -864,9 +861,9 @@
       <c r="D24" s="10">
         <v>23</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="26"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="23"/>
       <c r="H24"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
@@ -877,9 +874,9 @@
       <c r="D25" s="5">
         <v>24</v>
       </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="26"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="23"/>
       <c r="H25"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
@@ -890,9 +887,9 @@
       <c r="D26" s="10">
         <v>25</v>
       </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="26"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="23"/>
       <c r="H26"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
@@ -903,9 +900,9 @@
       <c r="D27" s="5">
         <v>26</v>
       </c>
-      <c r="E27" s="26"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="26"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="23"/>
       <c r="H27"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
@@ -916,9 +913,9 @@
       <c r="D28" s="10">
         <v>27</v>
       </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="26"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="23"/>
       <c r="H28"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
@@ -929,35 +926,35 @@
       <c r="D29" s="5">
         <v>28</v>
       </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="26"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="23"/>
       <c r="H29"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="20"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="10">
         <v>29</v>
       </c>
       <c r="D30" s="10">
         <v>29</v>
       </c>
-      <c r="E30" s="26"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="26"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="23"/>
       <c r="H30"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="22"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="5">
         <v>30</v>
       </c>
       <c r="D31" s="5">
         <v>30</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="26"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="23"/>
       <c r="H31"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
@@ -968,9 +965,9 @@
       <c r="D32" s="10">
         <v>31</v>
       </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="26"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="23"/>
       <c r="H32"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
@@ -981,9 +978,9 @@
       <c r="D33" s="5">
         <v>32</v>
       </c>
-      <c r="E33" s="26"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="26"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="23"/>
       <c r="H33"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
@@ -994,9 +991,9 @@
       <c r="D34" s="10">
         <v>33</v>
       </c>
-      <c r="E34" s="26"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="26"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="23"/>
       <c r="H34"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
@@ -1007,9 +1004,9 @@
       <c r="D35" s="5">
         <v>34</v>
       </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="26"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="23"/>
       <c r="H35"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
@@ -1020,9 +1017,9 @@
       <c r="D36" s="10">
         <v>35</v>
       </c>
-      <c r="E36" s="26"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="26"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="23"/>
       <c r="H36"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
@@ -1033,35 +1030,35 @@
       <c r="D37" s="5">
         <v>36</v>
       </c>
-      <c r="E37" s="26"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="26"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="23"/>
       <c r="H37"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="20"/>
+      <c r="B38" s="17"/>
       <c r="C38" s="10">
         <v>37</v>
       </c>
       <c r="D38" s="10">
         <v>37</v>
       </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="26"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="23"/>
       <c r="H38"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="22"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="5">
         <v>38</v>
       </c>
       <c r="D39" s="5">
         <v>38</v>
       </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="26"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="23"/>
       <c r="H39"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
@@ -1072,9 +1069,9 @@
       <c r="D40" s="10">
         <v>39</v>
       </c>
-      <c r="E40" s="26"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="26"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="23"/>
       <c r="H40"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
@@ -1085,9 +1082,9 @@
       <c r="D41" s="5">
         <v>40</v>
       </c>
-      <c r="E41" s="26"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="26"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="23"/>
       <c r="H41"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
@@ -1098,9 +1095,9 @@
       <c r="D42" s="10">
         <v>41</v>
       </c>
-      <c r="E42" s="26"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="26"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="23"/>
       <c r="H42"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">
@@ -1111,9 +1108,9 @@
       <c r="D43" s="5">
         <v>42</v>
       </c>
-      <c r="E43" s="26"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="26"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="23"/>
       <c r="H43"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.2">
@@ -1124,9 +1121,9 @@
       <c r="D44" s="10">
         <v>43</v>
       </c>
-      <c r="E44" s="26"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="26"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="23"/>
       <c r="H44"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
@@ -1137,9 +1134,9 @@
       <c r="D45" s="5">
         <v>44</v>
       </c>
-      <c r="E45" s="26"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="26"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="23"/>
       <c r="H45"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.2">
@@ -1150,9 +1147,9 @@
       <c r="D46" s="10">
         <v>45</v>
       </c>
-      <c r="E46" s="26"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="26"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="23"/>
       <c r="H46"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
@@ -1163,9 +1160,9 @@
       <c r="D47" s="5">
         <v>46</v>
       </c>
-      <c r="E47" s="26"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="26"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="23"/>
       <c r="H47"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.2">
@@ -1176,9 +1173,9 @@
       <c r="D48" s="10">
         <v>47</v>
       </c>
-      <c r="E48" s="26"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="26"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="23"/>
       <c r="H48"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
@@ -1189,9 +1186,9 @@
       <c r="D49" s="5">
         <v>48</v>
       </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="26"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="23"/>
       <c r="H49"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.2">
@@ -1202,9 +1199,9 @@
       <c r="D50" s="10">
         <v>49</v>
       </c>
-      <c r="E50" s="26"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="26"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="23"/>
       <c r="H50"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
@@ -1215,9 +1212,9 @@
       <c r="D51" s="5">
         <v>50</v>
       </c>
-      <c r="E51" s="26"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="26"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="23"/>
       <c r="H51"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.2">
@@ -1228,9 +1225,9 @@
       <c r="D52" s="10">
         <v>51</v>
       </c>
-      <c r="E52" s="26"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="26"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="23"/>
       <c r="H52"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
@@ -1241,35 +1238,35 @@
       <c r="D53" s="5">
         <v>52</v>
       </c>
-      <c r="E53" s="26"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="26"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="23"/>
       <c r="H53"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="20"/>
+      <c r="B54" s="17"/>
       <c r="C54" s="10">
         <v>53</v>
       </c>
       <c r="D54" s="10">
         <v>53</v>
       </c>
-      <c r="E54" s="26"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="26"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="23"/>
       <c r="H54"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="22"/>
+      <c r="B55" s="19"/>
       <c r="C55" s="5">
         <v>54</v>
       </c>
       <c r="D55" s="5">
         <v>54</v>
       </c>
-      <c r="E55" s="26"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="26"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="23"/>
       <c r="H55"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
@@ -1280,9 +1277,9 @@
       <c r="D56" s="10">
         <v>55</v>
       </c>
-      <c r="E56" s="26"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="26"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="23"/>
       <c r="H56"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.2">
@@ -1293,9 +1290,9 @@
       <c r="D57" s="5">
         <v>56</v>
       </c>
-      <c r="E57" s="26"/>
-      <c r="F57" s="23"/>
-      <c r="G57" s="26"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="23"/>
       <c r="H57"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.2">
@@ -1306,9 +1303,9 @@
       <c r="D58" s="10">
         <v>57</v>
       </c>
-      <c r="E58" s="26"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="26"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="23"/>
       <c r="H58"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.2">
@@ -1319,9 +1316,9 @@
       <c r="D59" s="5">
         <v>58</v>
       </c>
-      <c r="E59" s="26"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="26"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="23"/>
       <c r="H59"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
@@ -1332,9 +1329,9 @@
       <c r="D60" s="10">
         <v>59</v>
       </c>
-      <c r="E60" s="26"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="26"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="23"/>
       <c r="H60"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.2">
@@ -1345,9 +1342,9 @@
       <c r="D61" s="5">
         <v>60</v>
       </c>
-      <c r="E61" s="26"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="26"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="23"/>
       <c r="H61"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
@@ -1358,9 +1355,9 @@
       <c r="D62" s="10">
         <v>61</v>
       </c>
-      <c r="E62" s="26"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="26"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="23"/>
       <c r="H62"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.2">
@@ -1371,9 +1368,9 @@
       <c r="D63" s="5">
         <v>62</v>
       </c>
-      <c r="E63" s="26"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="26"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="23"/>
       <c r="H63"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
@@ -1384,9 +1381,9 @@
       <c r="D64" s="10">
         <v>63</v>
       </c>
-      <c r="E64" s="26"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="26"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="23"/>
       <c r="H64"/>
     </row>
     <row r="65" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1397,10 +1394,10 @@
       <c r="D65" s="5">
         <v>64</v>
       </c>
-      <c r="E65" s="26"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="26"/>
-      <c r="H65" s="26"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="23"/>
     </row>
     <row r="66" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B66" s="11"/>
@@ -1410,9 +1407,9 @@
       <c r="D66" s="10">
         <v>65</v>
       </c>
-      <c r="E66" s="26"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="26"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="23"/>
       <c r="H66"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
@@ -1423,9 +1420,9 @@
       <c r="D67" s="5">
         <v>66</v>
       </c>
-      <c r="E67" s="26"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="26"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="23"/>
       <c r="H67"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
@@ -1436,9 +1433,9 @@
       <c r="D68" s="10">
         <v>67</v>
       </c>
-      <c r="E68" s="26"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="26"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="23"/>
       <c r="H68"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
@@ -1449,9 +1446,9 @@
       <c r="D69" s="5">
         <v>68</v>
       </c>
-      <c r="E69" s="26"/>
-      <c r="F69" s="23"/>
-      <c r="G69" s="26"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="23"/>
       <c r="H69"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
@@ -1462,9 +1459,9 @@
       <c r="D70" s="10">
         <v>69</v>
       </c>
-      <c r="E70" s="26"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="26"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="23"/>
       <c r="H70"/>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.2">
@@ -1475,9 +1472,9 @@
       <c r="D71" s="5">
         <v>70</v>
       </c>
-      <c r="E71" s="26"/>
-      <c r="F71" s="23"/>
-      <c r="G71" s="26"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="23"/>
       <c r="H71"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.2">
@@ -1488,9 +1485,9 @@
       <c r="D72" s="10">
         <v>71</v>
       </c>
-      <c r="E72" s="26"/>
-      <c r="F72" s="23"/>
-      <c r="G72" s="26"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="23"/>
       <c r="H72"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.2">
@@ -1501,35 +1498,35 @@
       <c r="D73" s="5">
         <v>72</v>
       </c>
-      <c r="E73" s="26"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="26"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="23"/>
       <c r="H73"/>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B74" s="20"/>
+      <c r="B74" s="17"/>
       <c r="C74" s="10">
         <v>73</v>
       </c>
       <c r="D74" s="10">
         <v>73</v>
       </c>
-      <c r="E74" s="26"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="26"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="23"/>
       <c r="H74"/>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B75" s="22"/>
+      <c r="B75" s="19"/>
       <c r="C75" s="5">
         <v>74</v>
       </c>
       <c r="D75" s="5">
         <v>74</v>
       </c>
-      <c r="E75" s="26"/>
-      <c r="F75" s="23"/>
-      <c r="G75" s="26"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="23"/>
       <c r="H75"/>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.2">
@@ -1540,9 +1537,9 @@
       <c r="D76" s="10">
         <v>75</v>
       </c>
-      <c r="E76" s="26"/>
-      <c r="F76" s="23"/>
-      <c r="G76" s="26"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="23"/>
       <c r="H76"/>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.2">
@@ -1553,9 +1550,9 @@
       <c r="D77" s="5">
         <v>76</v>
       </c>
-      <c r="E77" s="26"/>
-      <c r="F77" s="23"/>
-      <c r="G77" s="26"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="23"/>
       <c r="H77"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.2">
@@ -1566,9 +1563,9 @@
       <c r="D78" s="10">
         <v>77</v>
       </c>
-      <c r="E78" s="26"/>
-      <c r="F78" s="23"/>
-      <c r="G78" s="26"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="23"/>
       <c r="H78"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.2">
@@ -1579,9 +1576,9 @@
       <c r="D79" s="5">
         <v>78</v>
       </c>
-      <c r="E79" s="26"/>
-      <c r="F79" s="23"/>
-      <c r="G79" s="26"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="23"/>
       <c r="H79"/>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.2">
@@ -1592,9 +1589,9 @@
       <c r="D80" s="10">
         <v>79</v>
       </c>
-      <c r="E80" s="26"/>
-      <c r="F80" s="23"/>
-      <c r="G80" s="26"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="23"/>
       <c r="H80"/>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.2">
@@ -1605,9 +1602,9 @@
       <c r="D81" s="5">
         <v>80</v>
       </c>
-      <c r="E81" s="26"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="26"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="23"/>
       <c r="H81"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.2">
@@ -1618,9 +1615,9 @@
       <c r="D82" s="10">
         <v>81</v>
       </c>
-      <c r="E82" s="26"/>
-      <c r="F82" s="23"/>
-      <c r="G82" s="26"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="23"/>
       <c r="H82"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.2">
@@ -1631,9 +1628,9 @@
       <c r="D83" s="5">
         <v>82</v>
       </c>
-      <c r="E83" s="26"/>
-      <c r="F83" s="23"/>
-      <c r="G83" s="26"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="23"/>
       <c r="H83"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.2">
@@ -1644,9 +1641,9 @@
       <c r="D84" s="10">
         <v>83</v>
       </c>
-      <c r="E84" s="26"/>
-      <c r="F84" s="23"/>
-      <c r="G84" s="26"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="23"/>
       <c r="H84"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.2">
@@ -1657,9 +1654,9 @@
       <c r="D85" s="5">
         <v>84</v>
       </c>
-      <c r="E85" s="26"/>
-      <c r="F85" s="23"/>
-      <c r="G85" s="26"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="23"/>
       <c r="H85"/>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.2">
@@ -1670,9 +1667,9 @@
       <c r="D86" s="10">
         <v>85</v>
       </c>
-      <c r="E86" s="26"/>
-      <c r="F86" s="23"/>
-      <c r="G86" s="26"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="23"/>
       <c r="H86"/>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.2">
@@ -1683,9 +1680,9 @@
       <c r="D87" s="5">
         <v>86</v>
       </c>
-      <c r="E87" s="26"/>
-      <c r="F87" s="23"/>
-      <c r="G87" s="26"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="23"/>
       <c r="H87"/>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.2">
@@ -1696,9 +1693,9 @@
       <c r="D88" s="10">
         <v>87</v>
       </c>
-      <c r="E88" s="26"/>
-      <c r="F88" s="23"/>
-      <c r="G88" s="26"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="23"/>
       <c r="H88"/>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.2">
@@ -1709,35 +1706,35 @@
       <c r="D89" s="5">
         <v>88</v>
       </c>
-      <c r="E89" s="26"/>
-      <c r="F89" s="23"/>
-      <c r="G89" s="26"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="23"/>
       <c r="H89"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B90" s="20"/>
+      <c r="B90" s="17"/>
       <c r="C90" s="10">
         <v>89</v>
       </c>
       <c r="D90" s="10">
         <v>89</v>
       </c>
-      <c r="E90" s="26"/>
-      <c r="F90" s="23"/>
-      <c r="G90" s="26"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="23"/>
       <c r="H90"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B91" s="22"/>
+      <c r="B91" s="19"/>
       <c r="C91" s="5">
         <v>90</v>
       </c>
       <c r="D91" s="5">
         <v>90</v>
       </c>
-      <c r="E91" s="26"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="26"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="23"/>
       <c r="H91"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.2">
@@ -1748,9 +1745,9 @@
       <c r="D92" s="10">
         <v>91</v>
       </c>
-      <c r="E92" s="26"/>
-      <c r="F92" s="23"/>
-      <c r="G92" s="26"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="23"/>
       <c r="H92"/>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.2">
@@ -1761,9 +1758,9 @@
       <c r="D93" s="5">
         <v>92</v>
       </c>
-      <c r="E93" s="26"/>
-      <c r="F93" s="23"/>
-      <c r="G93" s="26"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="23"/>
       <c r="H93"/>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.2">
@@ -1774,9 +1771,9 @@
       <c r="D94" s="10">
         <v>93</v>
       </c>
-      <c r="E94" s="26"/>
-      <c r="F94" s="23"/>
-      <c r="G94" s="26"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="23"/>
       <c r="H94"/>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.2">
@@ -1787,9 +1784,9 @@
       <c r="D95" s="5">
         <v>94</v>
       </c>
-      <c r="E95" s="26"/>
-      <c r="F95" s="23"/>
-      <c r="G95" s="26"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="23"/>
       <c r="H95"/>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.2">
@@ -1800,9 +1797,9 @@
       <c r="D96" s="10">
         <v>95</v>
       </c>
-      <c r="E96" s="26"/>
-      <c r="F96" s="23"/>
-      <c r="G96" s="26"/>
+      <c r="E96" s="23"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="23"/>
       <c r="H96"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.2">
@@ -1813,9 +1810,9 @@
       <c r="D97" s="5">
         <v>96</v>
       </c>
-      <c r="E97" s="26"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="26"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="23"/>
       <c r="H97"/>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.2">
@@ -1826,9 +1823,9 @@
       <c r="D98" s="10">
         <v>97</v>
       </c>
-      <c r="E98" s="26"/>
-      <c r="F98" s="23"/>
-      <c r="G98" s="26"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="23"/>
       <c r="H98"/>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.2">
@@ -1839,9 +1836,9 @@
       <c r="D99" s="5">
         <v>98</v>
       </c>
-      <c r="E99" s="26"/>
-      <c r="F99" s="23"/>
-      <c r="G99" s="26"/>
+      <c r="E99" s="23"/>
+      <c r="F99" s="20"/>
+      <c r="G99" s="23"/>
       <c r="H99"/>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.2">
@@ -1852,9 +1849,9 @@
       <c r="D100" s="10">
         <v>99</v>
       </c>
-      <c r="E100" s="26"/>
-      <c r="F100" s="23"/>
-      <c r="G100" s="26"/>
+      <c r="E100" s="23"/>
+      <c r="F100" s="20"/>
+      <c r="G100" s="23"/>
       <c r="H100"/>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.2">
@@ -1865,35 +1862,35 @@
       <c r="D101" s="5">
         <v>100</v>
       </c>
-      <c r="E101" s="26"/>
-      <c r="F101" s="23"/>
-      <c r="G101" s="26"/>
+      <c r="E101" s="23"/>
+      <c r="F101" s="20"/>
+      <c r="G101" s="23"/>
       <c r="H101"/>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B102" s="20"/>
+      <c r="B102" s="17"/>
       <c r="C102" s="10">
         <v>101</v>
       </c>
       <c r="D102" s="10">
         <v>101</v>
       </c>
-      <c r="E102" s="26"/>
-      <c r="F102" s="23"/>
-      <c r="G102" s="26"/>
+      <c r="E102" s="23"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="23"/>
       <c r="H102"/>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B103" s="22"/>
+      <c r="B103" s="19"/>
       <c r="C103" s="5">
         <v>102</v>
       </c>
       <c r="D103" s="5">
         <v>102</v>
       </c>
-      <c r="E103" s="26"/>
-      <c r="F103" s="23"/>
-      <c r="G103" s="26"/>
+      <c r="E103" s="23"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="23"/>
       <c r="H103"/>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.2">
@@ -1904,9 +1901,9 @@
       <c r="D104" s="10">
         <v>103</v>
       </c>
-      <c r="E104" s="26"/>
-      <c r="F104" s="23"/>
-      <c r="G104" s="26"/>
+      <c r="E104" s="23"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="23"/>
       <c r="H104"/>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.2">
@@ -1917,9 +1914,9 @@
       <c r="D105" s="5">
         <v>104</v>
       </c>
-      <c r="E105" s="26"/>
-      <c r="F105" s="23"/>
-      <c r="G105" s="26"/>
+      <c r="E105" s="23"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="23"/>
       <c r="H105"/>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.2">
@@ -1930,9 +1927,9 @@
       <c r="D106" s="10">
         <v>105</v>
       </c>
-      <c r="E106" s="26"/>
-      <c r="F106" s="23"/>
-      <c r="G106" s="26"/>
+      <c r="E106" s="23"/>
+      <c r="F106" s="20"/>
+      <c r="G106" s="23"/>
       <c r="H106"/>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.2">
@@ -1943,9 +1940,9 @@
       <c r="D107" s="5">
         <v>106</v>
       </c>
-      <c r="E107" s="26"/>
-      <c r="F107" s="23"/>
-      <c r="G107" s="26"/>
+      <c r="E107" s="23"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="23"/>
       <c r="H107"/>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.2">
@@ -1956,9 +1953,9 @@
       <c r="D108" s="10">
         <v>107</v>
       </c>
-      <c r="E108" s="26"/>
-      <c r="F108" s="23"/>
-      <c r="G108" s="26"/>
+      <c r="E108" s="23"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="23"/>
       <c r="H108"/>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.2">
@@ -1969,9 +1966,9 @@
       <c r="D109" s="5">
         <v>108</v>
       </c>
-      <c r="E109" s="26"/>
-      <c r="F109" s="23"/>
-      <c r="G109" s="26"/>
+      <c r="E109" s="23"/>
+      <c r="F109" s="20"/>
+      <c r="G109" s="23"/>
       <c r="H109"/>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.2">
@@ -1982,9 +1979,9 @@
       <c r="D110" s="10">
         <v>109</v>
       </c>
-      <c r="E110" s="26"/>
-      <c r="F110" s="23"/>
-      <c r="G110" s="26"/>
+      <c r="E110" s="23"/>
+      <c r="F110" s="20"/>
+      <c r="G110" s="23"/>
       <c r="H110"/>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.2">
@@ -1995,9 +1992,9 @@
       <c r="D111" s="5">
         <v>110</v>
       </c>
-      <c r="E111" s="26"/>
-      <c r="F111" s="23"/>
-      <c r="G111" s="26"/>
+      <c r="E111" s="23"/>
+      <c r="F111" s="20"/>
+      <c r="G111" s="23"/>
       <c r="H111"/>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.2">
@@ -2008,9 +2005,9 @@
       <c r="D112" s="10">
         <v>111</v>
       </c>
-      <c r="E112" s="26"/>
-      <c r="F112" s="23"/>
-      <c r="G112" s="26"/>
+      <c r="E112" s="23"/>
+      <c r="F112" s="20"/>
+      <c r="G112" s="23"/>
       <c r="H112"/>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.2">
@@ -2021,9 +2018,9 @@
       <c r="D113" s="5">
         <v>112</v>
       </c>
-      <c r="E113" s="26"/>
-      <c r="F113" s="23"/>
-      <c r="G113" s="26"/>
+      <c r="E113" s="23"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="23"/>
       <c r="H113"/>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.2">
@@ -2034,9 +2031,9 @@
       <c r="D114" s="10">
         <v>113</v>
       </c>
-      <c r="E114" s="26"/>
-      <c r="F114" s="23"/>
-      <c r="G114" s="26"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="20"/>
+      <c r="G114" s="23"/>
       <c r="H114"/>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.2">
@@ -2047,9 +2044,9 @@
       <c r="D115" s="5">
         <v>114</v>
       </c>
-      <c r="E115" s="26"/>
-      <c r="F115" s="23"/>
-      <c r="G115" s="26"/>
+      <c r="E115" s="23"/>
+      <c r="F115" s="20"/>
+      <c r="G115" s="23"/>
       <c r="H115"/>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.2">
@@ -2060,9 +2057,9 @@
       <c r="D116" s="10">
         <v>115</v>
       </c>
-      <c r="E116" s="26"/>
-      <c r="F116" s="23"/>
-      <c r="G116" s="26"/>
+      <c r="E116" s="23"/>
+      <c r="F116" s="20"/>
+      <c r="G116" s="23"/>
       <c r="H116"/>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.2">
@@ -2073,35 +2070,35 @@
       <c r="D117" s="5">
         <v>116</v>
       </c>
-      <c r="E117" s="26"/>
-      <c r="F117" s="23"/>
-      <c r="G117" s="26"/>
+      <c r="E117" s="23"/>
+      <c r="F117" s="20"/>
+      <c r="G117" s="23"/>
       <c r="H117"/>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B118" s="20"/>
+      <c r="B118" s="17"/>
       <c r="C118" s="10">
         <v>117</v>
       </c>
       <c r="D118" s="10">
         <v>117</v>
       </c>
-      <c r="E118" s="26"/>
-      <c r="F118" s="23"/>
-      <c r="G118" s="26"/>
+      <c r="E118" s="23"/>
+      <c r="F118" s="20"/>
+      <c r="G118" s="23"/>
       <c r="H118"/>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B119" s="22"/>
+      <c r="B119" s="19"/>
       <c r="C119" s="5">
         <v>118</v>
       </c>
       <c r="D119" s="5">
         <v>118</v>
       </c>
-      <c r="E119" s="26"/>
-      <c r="F119" s="23"/>
-      <c r="G119" s="26"/>
+      <c r="E119" s="23"/>
+      <c r="F119" s="20"/>
+      <c r="G119" s="23"/>
       <c r="H119"/>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.2">
@@ -2112,9 +2109,9 @@
       <c r="D120" s="10">
         <v>119</v>
       </c>
-      <c r="E120" s="26"/>
-      <c r="F120" s="23"/>
-      <c r="G120" s="26"/>
+      <c r="E120" s="23"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="23"/>
       <c r="H120"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.2">
@@ -2125,9 +2122,9 @@
       <c r="D121" s="5">
         <v>120</v>
       </c>
-      <c r="E121" s="26"/>
-      <c r="F121" s="23"/>
-      <c r="G121" s="26"/>
+      <c r="E121" s="23"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="23"/>
       <c r="H121"/>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.2">
@@ -2138,9 +2135,9 @@
       <c r="D122" s="10">
         <v>121</v>
       </c>
-      <c r="E122" s="26"/>
-      <c r="F122" s="23"/>
-      <c r="G122" s="26"/>
+      <c r="E122" s="23"/>
+      <c r="F122" s="20"/>
+      <c r="G122" s="23"/>
       <c r="H122"/>
     </row>
     <row r="123" spans="2:8" x14ac:dyDescent="0.2">
@@ -2151,9 +2148,9 @@
       <c r="D123" s="5">
         <v>122</v>
       </c>
-      <c r="E123" s="26"/>
-      <c r="F123" s="23"/>
-      <c r="G123" s="26"/>
+      <c r="E123" s="23"/>
+      <c r="F123" s="20"/>
+      <c r="G123" s="23"/>
       <c r="H123"/>
     </row>
     <row r="124" spans="2:8" x14ac:dyDescent="0.2">
@@ -2164,9 +2161,9 @@
       <c r="D124" s="10">
         <v>123</v>
       </c>
-      <c r="E124" s="26"/>
-      <c r="F124" s="23"/>
-      <c r="G124" s="26"/>
+      <c r="E124" s="23"/>
+      <c r="F124" s="20"/>
+      <c r="G124" s="23"/>
       <c r="H124"/>
     </row>
     <row r="125" spans="2:8" x14ac:dyDescent="0.2">
@@ -2177,9 +2174,9 @@
       <c r="D125" s="5">
         <v>124</v>
       </c>
-      <c r="E125" s="26"/>
-      <c r="F125" s="23"/>
-      <c r="G125" s="26"/>
+      <c r="E125" s="23"/>
+      <c r="F125" s="20"/>
+      <c r="G125" s="23"/>
       <c r="H125"/>
     </row>
     <row r="126" spans="2:8" x14ac:dyDescent="0.2">
@@ -2190,9 +2187,9 @@
       <c r="D126" s="10">
         <v>125</v>
       </c>
-      <c r="E126" s="26"/>
-      <c r="F126" s="23"/>
-      <c r="G126" s="26"/>
+      <c r="E126" s="23"/>
+      <c r="F126" s="20"/>
+      <c r="G126" s="23"/>
       <c r="H126"/>
     </row>
     <row r="127" spans="2:8" x14ac:dyDescent="0.2">
@@ -2203,9 +2200,9 @@
       <c r="D127" s="5">
         <v>126</v>
       </c>
-      <c r="E127" s="26"/>
-      <c r="F127" s="23"/>
-      <c r="G127" s="26"/>
+      <c r="E127" s="23"/>
+      <c r="F127" s="20"/>
+      <c r="G127" s="23"/>
       <c r="H127"/>
     </row>
     <row r="128" spans="2:8" x14ac:dyDescent="0.2">
@@ -2216,9 +2213,9 @@
       <c r="D128" s="10">
         <v>127</v>
       </c>
-      <c r="E128" s="26"/>
-      <c r="F128" s="23"/>
-      <c r="G128" s="26"/>
+      <c r="E128" s="23"/>
+      <c r="F128" s="20"/>
+      <c r="G128" s="23"/>
       <c r="H128"/>
     </row>
     <row r="129" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2229,10 +2226,10 @@
       <c r="D129" s="5">
         <v>128</v>
       </c>
-      <c r="E129" s="26"/>
-      <c r="F129" s="23"/>
-      <c r="G129" s="26"/>
-      <c r="H129" s="26"/>
+      <c r="E129" s="23"/>
+      <c r="F129" s="20"/>
+      <c r="G129" s="23"/>
+      <c r="H129" s="23"/>
     </row>
     <row r="130" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B130" s="6"/>
@@ -2242,9 +2239,9 @@
       <c r="D130" s="10">
         <v>129</v>
       </c>
-      <c r="E130" s="26"/>
-      <c r="F130" s="23"/>
-      <c r="G130" s="26"/>
+      <c r="E130" s="23"/>
+      <c r="F130" s="20"/>
+      <c r="G130" s="23"/>
       <c r="H130"/>
     </row>
     <row r="131" spans="2:8" x14ac:dyDescent="0.2">
@@ -2255,9 +2252,9 @@
       <c r="D131" s="5">
         <v>130</v>
       </c>
-      <c r="E131" s="26"/>
-      <c r="F131" s="23"/>
-      <c r="G131" s="26"/>
+      <c r="E131" s="23"/>
+      <c r="F131" s="20"/>
+      <c r="G131" s="23"/>
       <c r="H131"/>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.2">
@@ -2268,9 +2265,9 @@
       <c r="D132" s="10">
         <v>131</v>
       </c>
-      <c r="E132" s="26"/>
-      <c r="F132" s="23"/>
-      <c r="G132" s="26"/>
+      <c r="E132" s="23"/>
+      <c r="F132" s="20"/>
+      <c r="G132" s="23"/>
       <c r="H132"/>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.2">
@@ -2281,35 +2278,35 @@
       <c r="D133" s="5">
         <v>132</v>
       </c>
-      <c r="E133" s="26"/>
-      <c r="F133" s="23"/>
-      <c r="G133" s="26"/>
+      <c r="E133" s="23"/>
+      <c r="F133" s="20"/>
+      <c r="G133" s="23"/>
       <c r="H133"/>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B134" s="20"/>
+      <c r="B134" s="17"/>
       <c r="C134" s="10">
         <v>133</v>
       </c>
       <c r="D134" s="10">
         <v>133</v>
       </c>
-      <c r="E134" s="26"/>
-      <c r="F134" s="23"/>
-      <c r="G134" s="26"/>
+      <c r="E134" s="23"/>
+      <c r="F134" s="20"/>
+      <c r="G134" s="23"/>
       <c r="H134"/>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B135" s="22"/>
+      <c r="B135" s="19"/>
       <c r="C135" s="5">
         <v>134</v>
       </c>
       <c r="D135" s="5">
         <v>134</v>
       </c>
-      <c r="E135" s="26"/>
-      <c r="F135" s="23"/>
-      <c r="G135" s="26"/>
+      <c r="E135" s="23"/>
+      <c r="F135" s="20"/>
+      <c r="G135" s="23"/>
       <c r="H135"/>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.2">
@@ -2320,9 +2317,9 @@
       <c r="D136" s="10">
         <v>135</v>
       </c>
-      <c r="E136" s="26"/>
-      <c r="F136" s="23"/>
-      <c r="G136" s="26"/>
+      <c r="E136" s="23"/>
+      <c r="F136" s="20"/>
+      <c r="G136" s="23"/>
       <c r="H136"/>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.2">
@@ -2333,9 +2330,9 @@
       <c r="D137" s="5">
         <v>136</v>
       </c>
-      <c r="E137" s="26"/>
-      <c r="F137" s="23"/>
-      <c r="G137" s="26"/>
+      <c r="E137" s="23"/>
+      <c r="F137" s="20"/>
+      <c r="G137" s="23"/>
       <c r="H137"/>
     </row>
     <row r="138" spans="2:8" x14ac:dyDescent="0.2">
@@ -2346,9 +2343,9 @@
       <c r="D138" s="10">
         <v>137</v>
       </c>
-      <c r="E138" s="26"/>
-      <c r="F138" s="23"/>
-      <c r="G138" s="26"/>
+      <c r="E138" s="23"/>
+      <c r="F138" s="20"/>
+      <c r="G138" s="23"/>
       <c r="H138"/>
     </row>
     <row r="139" spans="2:8" x14ac:dyDescent="0.2">
@@ -2359,9 +2356,9 @@
       <c r="D139" s="5">
         <v>138</v>
       </c>
-      <c r="E139" s="26"/>
-      <c r="F139" s="23"/>
-      <c r="G139" s="26"/>
+      <c r="E139" s="23"/>
+      <c r="F139" s="20"/>
+      <c r="G139" s="23"/>
       <c r="H139"/>
     </row>
     <row r="140" spans="2:8" x14ac:dyDescent="0.2">
@@ -2372,9 +2369,9 @@
       <c r="D140" s="10">
         <v>139</v>
       </c>
-      <c r="E140" s="26"/>
-      <c r="F140" s="23"/>
-      <c r="G140" s="26"/>
+      <c r="E140" s="23"/>
+      <c r="F140" s="20"/>
+      <c r="G140" s="23"/>
       <c r="H140"/>
     </row>
     <row r="141" spans="2:8" x14ac:dyDescent="0.2">
@@ -2385,9 +2382,9 @@
       <c r="D141" s="5">
         <v>140</v>
       </c>
-      <c r="E141" s="26"/>
-      <c r="F141" s="23"/>
-      <c r="G141" s="26"/>
+      <c r="E141" s="23"/>
+      <c r="F141" s="20"/>
+      <c r="G141" s="23"/>
       <c r="H141"/>
     </row>
     <row r="142" spans="2:8" x14ac:dyDescent="0.2">
@@ -2398,9 +2395,9 @@
       <c r="D142" s="10">
         <v>141</v>
       </c>
-      <c r="E142" s="26"/>
-      <c r="F142" s="23"/>
-      <c r="G142" s="26"/>
+      <c r="E142" s="23"/>
+      <c r="F142" s="20"/>
+      <c r="G142" s="23"/>
       <c r="H142"/>
     </row>
     <row r="143" spans="2:8" x14ac:dyDescent="0.2">
@@ -2411,9 +2408,9 @@
       <c r="D143" s="5">
         <v>142</v>
       </c>
-      <c r="E143" s="26"/>
-      <c r="F143" s="23"/>
-      <c r="G143" s="26"/>
+      <c r="E143" s="23"/>
+      <c r="F143" s="20"/>
+      <c r="G143" s="23"/>
       <c r="H143"/>
     </row>
     <row r="144" spans="2:8" x14ac:dyDescent="0.2">
@@ -2424,9 +2421,9 @@
       <c r="D144" s="10">
         <v>143</v>
       </c>
-      <c r="E144" s="26"/>
-      <c r="F144" s="23"/>
-      <c r="G144" s="26"/>
+      <c r="E144" s="23"/>
+      <c r="F144" s="20"/>
+      <c r="G144" s="23"/>
       <c r="H144"/>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.2">
@@ -2437,9 +2434,9 @@
       <c r="D145" s="5">
         <v>144</v>
       </c>
-      <c r="E145" s="26"/>
-      <c r="F145" s="23"/>
-      <c r="G145" s="26"/>
+      <c r="E145" s="23"/>
+      <c r="F145" s="20"/>
+      <c r="G145" s="23"/>
       <c r="H145"/>
     </row>
     <row r="146" spans="2:8" x14ac:dyDescent="0.2">
@@ -2450,9 +2447,9 @@
       <c r="D146" s="10">
         <v>145</v>
       </c>
-      <c r="E146" s="26"/>
-      <c r="F146" s="23"/>
-      <c r="G146" s="26"/>
+      <c r="E146" s="23"/>
+      <c r="F146" s="20"/>
+      <c r="G146" s="23"/>
       <c r="H146"/>
     </row>
     <row r="147" spans="2:8" x14ac:dyDescent="0.2">
@@ -2463,9 +2460,9 @@
       <c r="D147" s="5">
         <v>146</v>
       </c>
-      <c r="E147" s="26"/>
-      <c r="F147" s="23"/>
-      <c r="G147" s="26"/>
+      <c r="E147" s="23"/>
+      <c r="F147" s="20"/>
+      <c r="G147" s="23"/>
       <c r="H147"/>
     </row>
     <row r="148" spans="2:8" x14ac:dyDescent="0.2">
@@ -2475,9 +2472,9 @@
       <c r="D148" s="10">
         <v>147</v>
       </c>
-      <c r="E148" s="26"/>
-      <c r="F148" s="23"/>
-      <c r="G148" s="26"/>
+      <c r="E148" s="23"/>
+      <c r="F148" s="20"/>
+      <c r="G148" s="23"/>
       <c r="H148"/>
     </row>
     <row r="149" spans="2:8" x14ac:dyDescent="0.2">
@@ -2487,22 +2484,22 @@
       <c r="D149" s="5">
         <v>148</v>
       </c>
-      <c r="E149" s="26"/>
-      <c r="F149" s="23"/>
-      <c r="G149" s="26"/>
+      <c r="E149" s="23"/>
+      <c r="F149" s="20"/>
+      <c r="G149" s="23"/>
       <c r="H149"/>
     </row>
     <row r="150" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B150" s="21"/>
+      <c r="B150" s="18"/>
       <c r="C150" s="10">
         <v>149</v>
       </c>
       <c r="D150" s="10">
         <v>149</v>
       </c>
-      <c r="E150" s="26"/>
-      <c r="F150" s="23"/>
-      <c r="G150" s="26"/>
+      <c r="E150" s="23"/>
+      <c r="F150" s="20"/>
+      <c r="G150" s="23"/>
       <c r="H150"/>
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.2">
@@ -2513,9 +2510,9 @@
       <c r="D151" s="5">
         <v>150</v>
       </c>
-      <c r="E151" s="26"/>
-      <c r="F151" s="23"/>
-      <c r="G151" s="26"/>
+      <c r="E151" s="23"/>
+      <c r="F151" s="20"/>
+      <c r="G151" s="23"/>
       <c r="H151"/>
     </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.2">
@@ -2526,9 +2523,9 @@
       <c r="D152" s="10">
         <v>151</v>
       </c>
-      <c r="E152" s="26"/>
-      <c r="F152" s="23"/>
-      <c r="G152" s="26"/>
+      <c r="E152" s="23"/>
+      <c r="F152" s="20"/>
+      <c r="G152" s="23"/>
       <c r="H152"/>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.2">
@@ -2538,9 +2535,9 @@
       <c r="D153" s="5">
         <v>152</v>
       </c>
-      <c r="E153" s="26"/>
-      <c r="F153" s="23"/>
-      <c r="G153" s="26"/>
+      <c r="E153" s="23"/>
+      <c r="F153" s="20"/>
+      <c r="G153" s="23"/>
       <c r="H153"/>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.2">
@@ -2550,9 +2547,9 @@
       <c r="D154" s="10">
         <v>153</v>
       </c>
-      <c r="E154" s="26"/>
-      <c r="F154" s="23"/>
-      <c r="G154" s="26"/>
+      <c r="E154" s="23"/>
+      <c r="F154" s="20"/>
+      <c r="G154" s="23"/>
       <c r="H154"/>
     </row>
     <row r="155" spans="2:8" x14ac:dyDescent="0.2">
@@ -2562,9 +2559,9 @@
       <c r="D155" s="5">
         <v>154</v>
       </c>
-      <c r="E155" s="26"/>
-      <c r="F155" s="23"/>
-      <c r="G155" s="26"/>
+      <c r="E155" s="23"/>
+      <c r="F155" s="20"/>
+      <c r="G155" s="23"/>
       <c r="H155"/>
     </row>
     <row r="156" spans="2:8" x14ac:dyDescent="0.2">
@@ -2574,9 +2571,9 @@
       <c r="D156" s="10">
         <v>155</v>
       </c>
-      <c r="E156" s="26"/>
-      <c r="F156" s="23"/>
-      <c r="G156" s="26"/>
+      <c r="E156" s="23"/>
+      <c r="F156" s="20"/>
+      <c r="G156" s="23"/>
       <c r="H156"/>
     </row>
     <row r="157" spans="2:8" x14ac:dyDescent="0.2">
@@ -2586,9 +2583,9 @@
       <c r="D157" s="5">
         <v>156</v>
       </c>
-      <c r="E157" s="26"/>
-      <c r="F157" s="23"/>
-      <c r="G157" s="26"/>
+      <c r="E157" s="23"/>
+      <c r="F157" s="20"/>
+      <c r="G157" s="23"/>
       <c r="H157"/>
     </row>
     <row r="158" spans="2:8" x14ac:dyDescent="0.2">
@@ -2598,9 +2595,9 @@
       <c r="D158" s="10">
         <v>157</v>
       </c>
-      <c r="E158" s="26"/>
-      <c r="F158" s="23"/>
-      <c r="G158" s="26"/>
+      <c r="E158" s="23"/>
+      <c r="F158" s="20"/>
+      <c r="G158" s="23"/>
       <c r="H158"/>
     </row>
     <row r="159" spans="2:8" x14ac:dyDescent="0.2">
@@ -2610,9 +2607,9 @@
       <c r="D159" s="5">
         <v>158</v>
       </c>
-      <c r="E159" s="26"/>
-      <c r="F159" s="23"/>
-      <c r="G159" s="26"/>
+      <c r="E159" s="23"/>
+      <c r="F159" s="20"/>
+      <c r="G159" s="23"/>
       <c r="H159"/>
     </row>
     <row r="160" spans="2:8" x14ac:dyDescent="0.2">
@@ -2622,9 +2619,9 @@
       <c r="D160" s="10">
         <v>159</v>
       </c>
-      <c r="E160" s="26"/>
-      <c r="F160" s="23"/>
-      <c r="G160" s="26"/>
+      <c r="E160" s="23"/>
+      <c r="F160" s="20"/>
+      <c r="G160" s="23"/>
       <c r="H160"/>
     </row>
     <row r="161" spans="2:8" x14ac:dyDescent="0.2">
@@ -2634,9 +2631,9 @@
       <c r="D161" s="5">
         <v>160</v>
       </c>
-      <c r="E161" s="26"/>
-      <c r="F161" s="23"/>
-      <c r="G161" s="26"/>
+      <c r="E161" s="23"/>
+      <c r="F161" s="20"/>
+      <c r="G161" s="23"/>
       <c r="H161"/>
     </row>
     <row r="162" spans="2:8" x14ac:dyDescent="0.2">
@@ -2646,9 +2643,9 @@
       <c r="D162" s="10">
         <v>161</v>
       </c>
-      <c r="E162" s="26"/>
-      <c r="F162" s="23"/>
-      <c r="G162" s="26"/>
+      <c r="E162" s="23"/>
+      <c r="F162" s="20"/>
+      <c r="G162" s="23"/>
       <c r="H162"/>
     </row>
     <row r="163" spans="2:8" x14ac:dyDescent="0.2">
@@ -2658,22 +2655,22 @@
       <c r="D163" s="5">
         <v>162</v>
       </c>
-      <c r="E163" s="26"/>
-      <c r="F163" s="23"/>
-      <c r="G163" s="26"/>
+      <c r="E163" s="23"/>
+      <c r="F163" s="20"/>
+      <c r="G163" s="23"/>
       <c r="H163"/>
     </row>
     <row r="164" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B164" s="21"/>
+      <c r="B164" s="18"/>
       <c r="C164" s="10">
         <v>163</v>
       </c>
       <c r="D164" s="10">
         <v>163</v>
       </c>
-      <c r="E164" s="26"/>
-      <c r="F164" s="23"/>
-      <c r="G164" s="26"/>
+      <c r="E164" s="23"/>
+      <c r="F164" s="20"/>
+      <c r="G164" s="23"/>
       <c r="H164"/>
     </row>
     <row r="165" spans="2:8" x14ac:dyDescent="0.2">
@@ -2684,9 +2681,9 @@
       <c r="D165" s="5">
         <v>164</v>
       </c>
-      <c r="E165" s="26"/>
-      <c r="F165" s="23"/>
-      <c r="G165" s="26"/>
+      <c r="E165" s="23"/>
+      <c r="F165" s="20"/>
+      <c r="G165" s="23"/>
       <c r="H165"/>
     </row>
     <row r="166" spans="2:8" x14ac:dyDescent="0.2">
@@ -2697,9 +2694,9 @@
       <c r="D166" s="10">
         <v>165</v>
       </c>
-      <c r="E166" s="26"/>
-      <c r="F166" s="23"/>
-      <c r="G166" s="26"/>
+      <c r="E166" s="23"/>
+      <c r="F166" s="20"/>
+      <c r="G166" s="23"/>
       <c r="H166"/>
     </row>
     <row r="167" spans="2:8" x14ac:dyDescent="0.2">
@@ -2709,9 +2706,9 @@
       <c r="D167" s="5">
         <v>166</v>
       </c>
-      <c r="E167" s="26"/>
-      <c r="F167" s="23"/>
-      <c r="G167" s="26"/>
+      <c r="E167" s="23"/>
+      <c r="F167" s="20"/>
+      <c r="G167" s="23"/>
       <c r="H167"/>
     </row>
     <row r="168" spans="2:8" x14ac:dyDescent="0.2">
@@ -2721,9 +2718,9 @@
       <c r="D168" s="10">
         <v>167</v>
       </c>
-      <c r="E168" s="26"/>
-      <c r="F168" s="23"/>
-      <c r="G168" s="26"/>
+      <c r="E168" s="23"/>
+      <c r="F168" s="20"/>
+      <c r="G168" s="23"/>
       <c r="H168"/>
     </row>
     <row r="169" spans="2:8" x14ac:dyDescent="0.2">
@@ -2733,9 +2730,9 @@
       <c r="D169" s="5">
         <v>168</v>
       </c>
-      <c r="E169" s="26"/>
-      <c r="F169" s="23"/>
-      <c r="G169" s="26"/>
+      <c r="E169" s="23"/>
+      <c r="F169" s="20"/>
+      <c r="G169" s="23"/>
       <c r="H169"/>
     </row>
     <row r="170" spans="2:8" x14ac:dyDescent="0.2">
@@ -2745,9 +2742,9 @@
       <c r="D170" s="10">
         <v>169</v>
       </c>
-      <c r="E170" s="26"/>
-      <c r="F170" s="23"/>
-      <c r="G170" s="26"/>
+      <c r="E170" s="23"/>
+      <c r="F170" s="20"/>
+      <c r="G170" s="23"/>
       <c r="H170"/>
     </row>
     <row r="171" spans="2:8" x14ac:dyDescent="0.2">
@@ -2757,9 +2754,9 @@
       <c r="D171" s="5">
         <v>170</v>
       </c>
-      <c r="E171" s="26"/>
-      <c r="F171" s="23"/>
-      <c r="G171" s="26"/>
+      <c r="E171" s="23"/>
+      <c r="F171" s="20"/>
+      <c r="G171" s="23"/>
       <c r="H171"/>
     </row>
     <row r="172" spans="2:8" x14ac:dyDescent="0.2">
@@ -2769,9 +2766,9 @@
       <c r="D172" s="10">
         <v>171</v>
       </c>
-      <c r="E172" s="26"/>
-      <c r="F172" s="23"/>
-      <c r="G172" s="26"/>
+      <c r="E172" s="23"/>
+      <c r="F172" s="20"/>
+      <c r="G172" s="23"/>
       <c r="H172"/>
     </row>
     <row r="173" spans="2:8" x14ac:dyDescent="0.2">
@@ -2781,9 +2778,9 @@
       <c r="D173" s="5">
         <v>172</v>
       </c>
-      <c r="E173" s="26"/>
-      <c r="F173" s="23"/>
-      <c r="G173" s="26"/>
+      <c r="E173" s="23"/>
+      <c r="F173" s="20"/>
+      <c r="G173" s="23"/>
       <c r="H173"/>
     </row>
     <row r="174" spans="2:8" x14ac:dyDescent="0.2">
@@ -2793,9 +2790,9 @@
       <c r="D174" s="10">
         <v>173</v>
       </c>
-      <c r="E174" s="26"/>
-      <c r="F174" s="23"/>
-      <c r="G174" s="26"/>
+      <c r="E174" s="23"/>
+      <c r="F174" s="20"/>
+      <c r="G174" s="23"/>
       <c r="H174"/>
     </row>
     <row r="175" spans="2:8" x14ac:dyDescent="0.2">
@@ -2805,9 +2802,9 @@
       <c r="D175" s="5">
         <v>174</v>
       </c>
-      <c r="E175" s="26"/>
-      <c r="F175" s="23"/>
-      <c r="G175" s="26"/>
+      <c r="E175" s="23"/>
+      <c r="F175" s="20"/>
+      <c r="G175" s="23"/>
       <c r="H175"/>
     </row>
     <row r="176" spans="2:8" x14ac:dyDescent="0.2">
@@ -2817,9 +2814,9 @@
       <c r="D176" s="10">
         <v>175</v>
       </c>
-      <c r="E176" s="26"/>
-      <c r="F176" s="23"/>
-      <c r="G176" s="26"/>
+      <c r="E176" s="23"/>
+      <c r="F176" s="20"/>
+      <c r="G176" s="23"/>
       <c r="H176"/>
     </row>
     <row r="177" spans="2:8" x14ac:dyDescent="0.2">
@@ -2829,9 +2826,9 @@
       <c r="D177" s="5">
         <v>176</v>
       </c>
-      <c r="E177" s="26"/>
-      <c r="F177" s="23"/>
-      <c r="G177" s="26"/>
+      <c r="E177" s="23"/>
+      <c r="F177" s="20"/>
+      <c r="G177" s="23"/>
       <c r="H177"/>
     </row>
     <row r="178" spans="2:8" x14ac:dyDescent="0.2">
@@ -2841,9 +2838,9 @@
       <c r="D178" s="10">
         <v>177</v>
       </c>
-      <c r="E178" s="26"/>
-      <c r="F178" s="23"/>
-      <c r="G178" s="26"/>
+      <c r="E178" s="23"/>
+      <c r="F178" s="20"/>
+      <c r="G178" s="23"/>
       <c r="H178"/>
     </row>
     <row r="179" spans="2:8" x14ac:dyDescent="0.2">
@@ -2853,22 +2850,22 @@
       <c r="D179" s="5">
         <v>178</v>
       </c>
-      <c r="E179" s="26"/>
-      <c r="F179" s="23"/>
-      <c r="G179" s="26"/>
+      <c r="E179" s="23"/>
+      <c r="F179" s="20"/>
+      <c r="G179" s="23"/>
       <c r="H179"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B180" s="21"/>
+      <c r="B180" s="18"/>
       <c r="C180" s="10">
         <v>179</v>
       </c>
       <c r="D180" s="10">
         <v>179</v>
       </c>
-      <c r="E180" s="26"/>
-      <c r="F180" s="23"/>
-      <c r="G180" s="26"/>
+      <c r="E180" s="23"/>
+      <c r="F180" s="20"/>
+      <c r="G180" s="23"/>
       <c r="H180"/>
     </row>
     <row r="181" spans="2:8" x14ac:dyDescent="0.2">
@@ -2879,9 +2876,9 @@
       <c r="D181" s="5">
         <v>180</v>
       </c>
-      <c r="E181" s="26"/>
-      <c r="F181" s="23"/>
-      <c r="G181" s="26"/>
+      <c r="E181" s="23"/>
+      <c r="F181" s="20"/>
+      <c r="G181" s="23"/>
       <c r="H181"/>
     </row>
     <row r="182" spans="2:8" x14ac:dyDescent="0.2">
@@ -2892,9 +2889,9 @@
       <c r="D182" s="10">
         <v>181</v>
       </c>
-      <c r="E182" s="26"/>
-      <c r="F182" s="23"/>
-      <c r="G182" s="26"/>
+      <c r="E182" s="23"/>
+      <c r="F182" s="20"/>
+      <c r="G182" s="23"/>
       <c r="H182"/>
     </row>
     <row r="183" spans="2:8" x14ac:dyDescent="0.2">
@@ -2904,9 +2901,9 @@
       <c r="D183" s="5">
         <v>182</v>
       </c>
-      <c r="E183" s="26"/>
-      <c r="F183" s="23"/>
-      <c r="G183" s="26"/>
+      <c r="E183" s="23"/>
+      <c r="F183" s="20"/>
+      <c r="G183" s="23"/>
       <c r="H183"/>
     </row>
     <row r="184" spans="2:8" x14ac:dyDescent="0.2">
@@ -2916,9 +2913,9 @@
       <c r="D184" s="10">
         <v>183</v>
       </c>
-      <c r="E184" s="26"/>
-      <c r="F184" s="23"/>
-      <c r="G184" s="26"/>
+      <c r="E184" s="23"/>
+      <c r="F184" s="20"/>
+      <c r="G184" s="23"/>
       <c r="H184"/>
     </row>
     <row r="185" spans="2:8" x14ac:dyDescent="0.2">
@@ -2928,9 +2925,9 @@
       <c r="D185" s="5">
         <v>184</v>
       </c>
-      <c r="E185" s="26"/>
-      <c r="F185" s="23"/>
-      <c r="G185" s="26"/>
+      <c r="E185" s="23"/>
+      <c r="F185" s="20"/>
+      <c r="G185" s="23"/>
       <c r="H185"/>
     </row>
     <row r="186" spans="2:8" x14ac:dyDescent="0.2">
@@ -2940,9 +2937,9 @@
       <c r="D186" s="10">
         <v>185</v>
       </c>
-      <c r="E186" s="26"/>
-      <c r="F186" s="23"/>
-      <c r="G186" s="26"/>
+      <c r="E186" s="23"/>
+      <c r="F186" s="20"/>
+      <c r="G186" s="23"/>
       <c r="H186"/>
     </row>
     <row r="187" spans="2:8" x14ac:dyDescent="0.2">
@@ -2952,9 +2949,9 @@
       <c r="D187" s="5">
         <v>186</v>
       </c>
-      <c r="E187" s="26"/>
-      <c r="F187" s="23"/>
-      <c r="G187" s="26"/>
+      <c r="E187" s="23"/>
+      <c r="F187" s="20"/>
+      <c r="G187" s="23"/>
       <c r="H187"/>
     </row>
     <row r="188" spans="2:8" x14ac:dyDescent="0.2">
@@ -2964,9 +2961,9 @@
       <c r="D188" s="10">
         <v>187</v>
       </c>
-      <c r="E188" s="26"/>
-      <c r="F188" s="23"/>
-      <c r="G188" s="26"/>
+      <c r="E188" s="23"/>
+      <c r="F188" s="20"/>
+      <c r="G188" s="23"/>
       <c r="H188"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.2">
@@ -2976,9 +2973,9 @@
       <c r="D189" s="5">
         <v>188</v>
       </c>
-      <c r="E189" s="26"/>
-      <c r="F189" s="23"/>
-      <c r="G189" s="26"/>
+      <c r="E189" s="23"/>
+      <c r="F189" s="20"/>
+      <c r="G189" s="23"/>
       <c r="H189"/>
     </row>
     <row r="190" spans="2:8" x14ac:dyDescent="0.2">
@@ -2988,9 +2985,9 @@
       <c r="D190" s="10">
         <v>189</v>
       </c>
-      <c r="E190" s="26"/>
-      <c r="F190" s="23"/>
-      <c r="G190" s="26"/>
+      <c r="E190" s="23"/>
+      <c r="F190" s="20"/>
+      <c r="G190" s="23"/>
       <c r="H190"/>
     </row>
     <row r="191" spans="2:8" x14ac:dyDescent="0.2">
@@ -3000,9 +2997,9 @@
       <c r="D191" s="5">
         <v>190</v>
       </c>
-      <c r="E191" s="26"/>
-      <c r="F191" s="23"/>
-      <c r="G191" s="26"/>
+      <c r="E191" s="23"/>
+      <c r="F191" s="20"/>
+      <c r="G191" s="23"/>
       <c r="H191"/>
     </row>
     <row r="192" spans="2:8" x14ac:dyDescent="0.2">
@@ -3012,9 +3009,9 @@
       <c r="D192" s="10">
         <v>191</v>
       </c>
-      <c r="E192" s="26"/>
-      <c r="F192" s="23"/>
-      <c r="G192" s="26"/>
+      <c r="E192" s="23"/>
+      <c r="F192" s="20"/>
+      <c r="G192" s="23"/>
       <c r="H192"/>
     </row>
     <row r="193" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3025,10 +3022,10 @@
       <c r="D193" s="5">
         <v>192</v>
       </c>
-      <c r="E193" s="26"/>
-      <c r="F193" s="23"/>
-      <c r="G193" s="26"/>
-      <c r="H193" s="26"/>
+      <c r="E193" s="23"/>
+      <c r="F193" s="20"/>
+      <c r="G193" s="23"/>
+      <c r="H193" s="23"/>
     </row>
     <row r="194" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C194" s="10">
@@ -3037,9 +3034,9 @@
       <c r="D194" s="10">
         <v>193</v>
       </c>
-      <c r="E194" s="26"/>
-      <c r="F194" s="23"/>
-      <c r="G194" s="26"/>
+      <c r="E194" s="23"/>
+      <c r="F194" s="20"/>
+      <c r="G194" s="23"/>
       <c r="H194"/>
     </row>
     <row r="195" spans="2:8" x14ac:dyDescent="0.2">
@@ -3049,22 +3046,22 @@
       <c r="D195" s="5">
         <v>194</v>
       </c>
-      <c r="E195" s="26"/>
-      <c r="F195" s="23"/>
-      <c r="G195" s="26"/>
+      <c r="E195" s="23"/>
+      <c r="F195" s="20"/>
+      <c r="G195" s="23"/>
       <c r="H195"/>
     </row>
     <row r="196" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B196" s="21"/>
+      <c r="B196" s="18"/>
       <c r="C196" s="10">
         <v>195</v>
       </c>
       <c r="D196" s="10">
         <v>195</v>
       </c>
-      <c r="E196" s="26"/>
-      <c r="F196" s="23"/>
-      <c r="G196" s="26"/>
+      <c r="E196" s="23"/>
+      <c r="F196" s="20"/>
+      <c r="G196" s="23"/>
       <c r="H196"/>
     </row>
     <row r="197" spans="2:8" x14ac:dyDescent="0.2">
@@ -3075,9 +3072,9 @@
       <c r="D197" s="5">
         <v>196</v>
       </c>
-      <c r="E197" s="26"/>
-      <c r="F197" s="23"/>
-      <c r="G197" s="26"/>
+      <c r="E197" s="23"/>
+      <c r="F197" s="20"/>
+      <c r="G197" s="23"/>
       <c r="H197"/>
     </row>
     <row r="198" spans="2:8" x14ac:dyDescent="0.2">
@@ -3088,9 +3085,9 @@
       <c r="D198" s="10">
         <v>197</v>
       </c>
-      <c r="E198" s="26"/>
-      <c r="F198" s="23"/>
-      <c r="G198" s="26"/>
+      <c r="E198" s="23"/>
+      <c r="F198" s="20"/>
+      <c r="G198" s="23"/>
       <c r="H198"/>
     </row>
     <row r="199" spans="2:8" x14ac:dyDescent="0.2">
@@ -3100,9 +3097,9 @@
       <c r="D199" s="5">
         <v>198</v>
       </c>
-      <c r="E199" s="26"/>
-      <c r="F199" s="23"/>
-      <c r="G199" s="26"/>
+      <c r="E199" s="23"/>
+      <c r="F199" s="20"/>
+      <c r="G199" s="23"/>
       <c r="H199"/>
     </row>
     <row r="200" spans="2:8" x14ac:dyDescent="0.2">
@@ -3112,9 +3109,9 @@
       <c r="D200" s="10">
         <v>199</v>
       </c>
-      <c r="E200" s="26"/>
-      <c r="F200" s="23"/>
-      <c r="G200" s="26"/>
+      <c r="E200" s="23"/>
+      <c r="F200" s="20"/>
+      <c r="G200" s="23"/>
       <c r="H200"/>
     </row>
     <row r="201" spans="2:8" x14ac:dyDescent="0.2">
@@ -3124,9 +3121,9 @@
       <c r="D201" s="5">
         <v>200</v>
       </c>
-      <c r="E201" s="26"/>
-      <c r="F201" s="23"/>
-      <c r="G201" s="26"/>
+      <c r="E201" s="23"/>
+      <c r="F201" s="20"/>
+      <c r="G201" s="23"/>
       <c r="H201"/>
     </row>
     <row r="202" spans="2:8" x14ac:dyDescent="0.2">
@@ -3136,9 +3133,9 @@
       <c r="D202" s="10">
         <v>201</v>
       </c>
-      <c r="E202" s="26"/>
-      <c r="F202" s="23"/>
-      <c r="G202" s="26"/>
+      <c r="E202" s="23"/>
+      <c r="F202" s="20"/>
+      <c r="G202" s="23"/>
       <c r="H202"/>
     </row>
     <row r="203" spans="2:8" x14ac:dyDescent="0.2">
@@ -3148,22 +3145,22 @@
       <c r="D203" s="5">
         <v>202</v>
       </c>
-      <c r="E203" s="26"/>
-      <c r="F203" s="23"/>
-      <c r="G203" s="26"/>
+      <c r="E203" s="23"/>
+      <c r="F203" s="20"/>
+      <c r="G203" s="23"/>
       <c r="H203"/>
     </row>
     <row r="204" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B204" s="21"/>
+      <c r="B204" s="18"/>
       <c r="C204" s="10">
         <v>203</v>
       </c>
       <c r="D204" s="10">
         <v>203</v>
       </c>
-      <c r="E204" s="26"/>
-      <c r="F204" s="23"/>
-      <c r="G204" s="26"/>
+      <c r="E204" s="23"/>
+      <c r="F204" s="20"/>
+      <c r="G204" s="23"/>
       <c r="H204"/>
     </row>
     <row r="205" spans="2:8" x14ac:dyDescent="0.2">
@@ -3174,9 +3171,9 @@
       <c r="D205" s="5">
         <v>204</v>
       </c>
-      <c r="E205" s="26"/>
-      <c r="F205" s="23"/>
-      <c r="G205" s="26"/>
+      <c r="E205" s="23"/>
+      <c r="F205" s="20"/>
+      <c r="G205" s="23"/>
       <c r="H205"/>
     </row>
     <row r="206" spans="2:8" x14ac:dyDescent="0.2">
@@ -3187,9 +3184,9 @@
       <c r="D206" s="10">
         <v>205</v>
       </c>
-      <c r="E206" s="26"/>
-      <c r="F206" s="23"/>
-      <c r="G206" s="26"/>
+      <c r="E206" s="23"/>
+      <c r="F206" s="20"/>
+      <c r="G206" s="23"/>
       <c r="H206"/>
     </row>
     <row r="207" spans="2:8" x14ac:dyDescent="0.2">
@@ -3199,9 +3196,9 @@
       <c r="D207" s="5">
         <v>206</v>
       </c>
-      <c r="E207" s="26"/>
-      <c r="F207" s="23"/>
-      <c r="G207" s="26"/>
+      <c r="E207" s="23"/>
+      <c r="F207" s="20"/>
+      <c r="G207" s="23"/>
       <c r="H207"/>
     </row>
     <row r="208" spans="2:8" x14ac:dyDescent="0.2">
@@ -3211,9 +3208,9 @@
       <c r="D208" s="10">
         <v>207</v>
       </c>
-      <c r="E208" s="26"/>
-      <c r="F208" s="23"/>
-      <c r="G208" s="26"/>
+      <c r="E208" s="23"/>
+      <c r="F208" s="20"/>
+      <c r="G208" s="23"/>
       <c r="H208"/>
     </row>
     <row r="209" spans="3:8" x14ac:dyDescent="0.2">
@@ -3223,9 +3220,9 @@
       <c r="D209" s="5">
         <v>208</v>
       </c>
-      <c r="E209" s="26"/>
-      <c r="F209" s="23"/>
-      <c r="G209" s="26"/>
+      <c r="E209" s="23"/>
+      <c r="F209" s="20"/>
+      <c r="G209" s="23"/>
       <c r="H209"/>
     </row>
     <row r="210" spans="3:8" x14ac:dyDescent="0.2">
@@ -3235,9 +3232,9 @@
       <c r="D210" s="10">
         <v>209</v>
       </c>
-      <c r="E210" s="26"/>
-      <c r="F210" s="23"/>
-      <c r="G210" s="26"/>
+      <c r="E210" s="23"/>
+      <c r="F210" s="20"/>
+      <c r="G210" s="23"/>
       <c r="H210"/>
     </row>
     <row r="211" spans="3:8" x14ac:dyDescent="0.2">
@@ -3247,9 +3244,9 @@
       <c r="D211" s="5">
         <v>210</v>
       </c>
-      <c r="E211" s="26"/>
-      <c r="F211" s="23"/>
-      <c r="G211" s="26"/>
+      <c r="E211" s="23"/>
+      <c r="F211" s="20"/>
+      <c r="G211" s="23"/>
       <c r="H211"/>
     </row>
     <row r="212" spans="3:8" x14ac:dyDescent="0.2">
@@ -3259,9 +3256,9 @@
       <c r="D212" s="10">
         <v>211</v>
       </c>
-      <c r="E212" s="26"/>
-      <c r="F212" s="23"/>
-      <c r="G212" s="26"/>
+      <c r="E212" s="23"/>
+      <c r="F212" s="20"/>
+      <c r="G212" s="23"/>
       <c r="H212"/>
     </row>
     <row r="213" spans="3:8" x14ac:dyDescent="0.2">
@@ -3271,9 +3268,9 @@
       <c r="D213" s="5">
         <v>212</v>
       </c>
-      <c r="E213" s="26"/>
-      <c r="F213" s="23"/>
-      <c r="G213" s="26"/>
+      <c r="E213" s="23"/>
+      <c r="F213" s="20"/>
+      <c r="G213" s="23"/>
       <c r="H213"/>
     </row>
     <row r="214" spans="3:8" x14ac:dyDescent="0.2">
@@ -3283,9 +3280,9 @@
       <c r="D214" s="10">
         <v>213</v>
       </c>
-      <c r="E214" s="26"/>
-      <c r="F214" s="23"/>
-      <c r="G214" s="26"/>
+      <c r="E214" s="23"/>
+      <c r="F214" s="20"/>
+      <c r="G214" s="23"/>
       <c r="H214"/>
     </row>
     <row r="215" spans="3:8" x14ac:dyDescent="0.2">
@@ -3295,9 +3292,9 @@
       <c r="D215" s="5">
         <v>214</v>
       </c>
-      <c r="E215" s="26"/>
-      <c r="F215" s="23"/>
-      <c r="G215" s="26"/>
+      <c r="E215" s="23"/>
+      <c r="F215" s="20"/>
+      <c r="G215" s="23"/>
       <c r="H215"/>
     </row>
     <row r="216" spans="3:8" x14ac:dyDescent="0.2">
@@ -3307,9 +3304,9 @@
       <c r="D216" s="10">
         <v>215</v>
       </c>
-      <c r="E216" s="26"/>
-      <c r="F216" s="23"/>
-      <c r="G216" s="26"/>
+      <c r="E216" s="23"/>
+      <c r="F216" s="20"/>
+      <c r="G216" s="23"/>
       <c r="H216"/>
     </row>
     <row r="217" spans="3:8" x14ac:dyDescent="0.2">
@@ -3319,9 +3316,9 @@
       <c r="D217" s="5">
         <v>216</v>
       </c>
-      <c r="E217" s="26"/>
-      <c r="F217" s="23"/>
-      <c r="G217" s="26"/>
+      <c r="E217" s="23"/>
+      <c r="F217" s="20"/>
+      <c r="G217" s="23"/>
       <c r="H217"/>
     </row>
     <row r="218" spans="3:8" x14ac:dyDescent="0.2">
@@ -3331,9 +3328,9 @@
       <c r="D218" s="10">
         <v>217</v>
       </c>
-      <c r="E218" s="26"/>
-      <c r="F218" s="23"/>
-      <c r="G218" s="26"/>
+      <c r="E218" s="23"/>
+      <c r="F218" s="20"/>
+      <c r="G218" s="23"/>
       <c r="H218"/>
     </row>
     <row r="219" spans="3:8" x14ac:dyDescent="0.2">
@@ -3343,9 +3340,9 @@
       <c r="D219" s="5">
         <v>218</v>
       </c>
-      <c r="E219" s="26"/>
-      <c r="F219" s="23"/>
-      <c r="G219" s="26"/>
+      <c r="E219" s="23"/>
+      <c r="F219" s="20"/>
+      <c r="G219" s="23"/>
       <c r="H219"/>
     </row>
     <row r="220" spans="3:8" x14ac:dyDescent="0.2">
@@ -3355,9 +3352,9 @@
       <c r="D220" s="10">
         <v>219</v>
       </c>
-      <c r="E220" s="26"/>
-      <c r="F220" s="23"/>
-      <c r="G220" s="26"/>
+      <c r="E220" s="23"/>
+      <c r="F220" s="20"/>
+      <c r="G220" s="23"/>
       <c r="H220"/>
     </row>
     <row r="221" spans="3:8" x14ac:dyDescent="0.2">
@@ -3367,9 +3364,9 @@
       <c r="D221" s="5">
         <v>220</v>
       </c>
-      <c r="E221" s="26"/>
-      <c r="F221" s="23"/>
-      <c r="G221" s="26"/>
+      <c r="E221" s="23"/>
+      <c r="F221" s="20"/>
+      <c r="G221" s="23"/>
       <c r="H221"/>
     </row>
     <row r="222" spans="3:8" x14ac:dyDescent="0.2">
@@ -3379,9 +3376,9 @@
       <c r="D222" s="10">
         <v>221</v>
       </c>
-      <c r="E222" s="26"/>
-      <c r="F222" s="23"/>
-      <c r="G222" s="26"/>
+      <c r="E222" s="23"/>
+      <c r="F222" s="20"/>
+      <c r="G222" s="23"/>
       <c r="H222"/>
     </row>
     <row r="223" spans="3:8" x14ac:dyDescent="0.2">
@@ -3391,9 +3388,9 @@
       <c r="D223" s="5">
         <v>222</v>
       </c>
-      <c r="E223" s="26"/>
-      <c r="F223" s="23"/>
-      <c r="G223" s="26"/>
+      <c r="E223" s="23"/>
+      <c r="F223" s="20"/>
+      <c r="G223" s="23"/>
       <c r="H223"/>
     </row>
     <row r="224" spans="3:8" x14ac:dyDescent="0.2">
@@ -3403,9 +3400,9 @@
       <c r="D224" s="10">
         <v>223</v>
       </c>
-      <c r="E224" s="26"/>
-      <c r="F224" s="23"/>
-      <c r="G224" s="26"/>
+      <c r="E224" s="23"/>
+      <c r="F224" s="20"/>
+      <c r="G224" s="23"/>
       <c r="H224"/>
     </row>
     <row r="225" spans="2:8" x14ac:dyDescent="0.2">
@@ -3415,9 +3412,9 @@
       <c r="D225" s="5">
         <v>224</v>
       </c>
-      <c r="E225" s="26"/>
-      <c r="F225" s="23"/>
-      <c r="G225" s="26"/>
+      <c r="E225" s="23"/>
+      <c r="F225" s="20"/>
+      <c r="G225" s="23"/>
       <c r="H225"/>
     </row>
     <row r="226" spans="2:8" x14ac:dyDescent="0.2">
@@ -3427,9 +3424,9 @@
       <c r="D226" s="10">
         <v>225</v>
       </c>
-      <c r="E226" s="26"/>
-      <c r="F226" s="23"/>
-      <c r="G226" s="26"/>
+      <c r="E226" s="23"/>
+      <c r="F226" s="20"/>
+      <c r="G226" s="23"/>
       <c r="H226"/>
     </row>
     <row r="227" spans="2:8" x14ac:dyDescent="0.2">
@@ -3439,9 +3436,9 @@
       <c r="D227" s="5">
         <v>226</v>
       </c>
-      <c r="E227" s="26"/>
-      <c r="F227" s="23"/>
-      <c r="G227" s="26"/>
+      <c r="E227" s="23"/>
+      <c r="F227" s="20"/>
+      <c r="G227" s="23"/>
       <c r="H227"/>
     </row>
     <row r="228" spans="2:8" x14ac:dyDescent="0.2">
@@ -3451,9 +3448,9 @@
       <c r="D228" s="10">
         <v>227</v>
       </c>
-      <c r="E228" s="26"/>
-      <c r="F228" s="23"/>
-      <c r="G228" s="26"/>
+      <c r="E228" s="23"/>
+      <c r="F228" s="20"/>
+      <c r="G228" s="23"/>
       <c r="H228"/>
     </row>
     <row r="229" spans="2:8" x14ac:dyDescent="0.2">
@@ -3463,9 +3460,9 @@
       <c r="D229" s="5">
         <v>228</v>
       </c>
-      <c r="E229" s="26"/>
-      <c r="F229" s="23"/>
-      <c r="G229" s="26"/>
+      <c r="E229" s="23"/>
+      <c r="F229" s="20"/>
+      <c r="G229" s="23"/>
       <c r="H229"/>
     </row>
     <row r="230" spans="2:8" x14ac:dyDescent="0.2">
@@ -3475,22 +3472,22 @@
       <c r="D230" s="10">
         <v>229</v>
       </c>
-      <c r="E230" s="26"/>
-      <c r="F230" s="23"/>
-      <c r="G230" s="26"/>
+      <c r="E230" s="23"/>
+      <c r="F230" s="20"/>
+      <c r="G230" s="23"/>
       <c r="H230"/>
     </row>
     <row r="231" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B231" s="21"/>
+      <c r="B231" s="18"/>
       <c r="C231" s="5">
         <v>230</v>
       </c>
       <c r="D231" s="5">
         <v>230</v>
       </c>
-      <c r="E231" s="26"/>
-      <c r="F231" s="23"/>
-      <c r="G231" s="26"/>
+      <c r="E231" s="23"/>
+      <c r="F231" s="20"/>
+      <c r="G231" s="23"/>
       <c r="H231"/>
     </row>
     <row r="232" spans="2:8" x14ac:dyDescent="0.2">
@@ -3501,9 +3498,9 @@
       <c r="D232" s="10">
         <v>231</v>
       </c>
-      <c r="E232" s="26"/>
-      <c r="F232" s="23"/>
-      <c r="G232" s="26"/>
+      <c r="E232" s="23"/>
+      <c r="F232" s="20"/>
+      <c r="G232" s="23"/>
       <c r="H232"/>
     </row>
     <row r="233" spans="2:8" x14ac:dyDescent="0.2">
@@ -3514,9 +3511,9 @@
       <c r="D233" s="5">
         <v>232</v>
       </c>
-      <c r="E233" s="26"/>
-      <c r="F233" s="23"/>
-      <c r="G233" s="26"/>
+      <c r="E233" s="23"/>
+      <c r="F233" s="20"/>
+      <c r="G233" s="23"/>
       <c r="H233"/>
     </row>
     <row r="234" spans="2:8" x14ac:dyDescent="0.2">
@@ -3526,9 +3523,9 @@
       <c r="D234" s="10">
         <v>233</v>
       </c>
-      <c r="E234" s="26"/>
-      <c r="F234" s="23"/>
-      <c r="G234" s="26"/>
+      <c r="E234" s="23"/>
+      <c r="F234" s="20"/>
+      <c r="G234" s="23"/>
       <c r="H234"/>
     </row>
     <row r="235" spans="2:8" x14ac:dyDescent="0.2">
@@ -3538,9 +3535,9 @@
       <c r="D235" s="5">
         <v>234</v>
       </c>
-      <c r="E235" s="26"/>
-      <c r="F235" s="23"/>
-      <c r="G235" s="26"/>
+      <c r="E235" s="23"/>
+      <c r="F235" s="20"/>
+      <c r="G235" s="23"/>
       <c r="H235"/>
     </row>
     <row r="236" spans="2:8" x14ac:dyDescent="0.2">
@@ -3550,9 +3547,9 @@
       <c r="D236" s="10">
         <v>235</v>
       </c>
-      <c r="E236" s="26"/>
-      <c r="F236" s="23"/>
-      <c r="G236" s="26"/>
+      <c r="E236" s="23"/>
+      <c r="F236" s="20"/>
+      <c r="G236" s="23"/>
       <c r="H236"/>
     </row>
     <row r="237" spans="2:8" x14ac:dyDescent="0.2">
@@ -3562,9 +3559,9 @@
       <c r="D237" s="5">
         <v>236</v>
       </c>
-      <c r="E237" s="26"/>
-      <c r="F237" s="23"/>
-      <c r="G237" s="26"/>
+      <c r="E237" s="23"/>
+      <c r="F237" s="20"/>
+      <c r="G237" s="23"/>
       <c r="H237"/>
     </row>
     <row r="238" spans="2:8" x14ac:dyDescent="0.2">
@@ -3574,9 +3571,9 @@
       <c r="D238" s="10">
         <v>237</v>
       </c>
-      <c r="E238" s="26"/>
-      <c r="F238" s="23"/>
-      <c r="G238" s="26"/>
+      <c r="E238" s="23"/>
+      <c r="F238" s="20"/>
+      <c r="G238" s="23"/>
       <c r="H238"/>
     </row>
     <row r="239" spans="2:8" x14ac:dyDescent="0.2">
@@ -3586,9 +3583,9 @@
       <c r="D239" s="5">
         <v>238</v>
       </c>
-      <c r="E239" s="26"/>
-      <c r="F239" s="23"/>
-      <c r="G239" s="26"/>
+      <c r="E239" s="23"/>
+      <c r="F239" s="20"/>
+      <c r="G239" s="23"/>
       <c r="H239"/>
     </row>
     <row r="240" spans="2:8" x14ac:dyDescent="0.2">
@@ -3598,9 +3595,9 @@
       <c r="D240" s="10">
         <v>239</v>
       </c>
-      <c r="E240" s="26"/>
-      <c r="F240" s="23"/>
-      <c r="G240" s="26"/>
+      <c r="E240" s="23"/>
+      <c r="F240" s="20"/>
+      <c r="G240" s="23"/>
       <c r="H240"/>
     </row>
     <row r="241" spans="2:8" x14ac:dyDescent="0.2">
@@ -3610,9 +3607,9 @@
       <c r="D241" s="5">
         <v>240</v>
       </c>
-      <c r="E241" s="26"/>
-      <c r="F241" s="23"/>
-      <c r="G241" s="26"/>
+      <c r="E241" s="23"/>
+      <c r="F241" s="20"/>
+      <c r="G241" s="23"/>
       <c r="H241"/>
     </row>
     <row r="242" spans="2:8" x14ac:dyDescent="0.2">
@@ -3622,9 +3619,9 @@
       <c r="D242" s="10">
         <v>241</v>
       </c>
-      <c r="E242" s="26"/>
-      <c r="F242" s="23"/>
-      <c r="G242" s="26"/>
+      <c r="E242" s="23"/>
+      <c r="F242" s="20"/>
+      <c r="G242" s="23"/>
       <c r="H242"/>
     </row>
     <row r="243" spans="2:8" x14ac:dyDescent="0.2">
@@ -3634,9 +3631,9 @@
       <c r="D243" s="5">
         <v>242</v>
       </c>
-      <c r="E243" s="26"/>
-      <c r="F243" s="23"/>
-      <c r="G243" s="26"/>
+      <c r="E243" s="23"/>
+      <c r="F243" s="20"/>
+      <c r="G243" s="23"/>
       <c r="H243"/>
     </row>
     <row r="244" spans="2:8" x14ac:dyDescent="0.2">
@@ -3646,9 +3643,9 @@
       <c r="D244" s="10">
         <v>243</v>
       </c>
-      <c r="E244" s="26"/>
-      <c r="F244" s="23"/>
-      <c r="G244" s="26"/>
+      <c r="E244" s="23"/>
+      <c r="F244" s="20"/>
+      <c r="G244" s="23"/>
       <c r="H244"/>
     </row>
     <row r="245" spans="2:8" x14ac:dyDescent="0.2">
@@ -3658,9 +3655,9 @@
       <c r="D245" s="5">
         <v>244</v>
       </c>
-      <c r="E245" s="26"/>
-      <c r="F245" s="23"/>
-      <c r="G245" s="26"/>
+      <c r="E245" s="23"/>
+      <c r="F245" s="20"/>
+      <c r="G245" s="23"/>
       <c r="H245"/>
     </row>
     <row r="246" spans="2:8" x14ac:dyDescent="0.2">
@@ -3670,9 +3667,9 @@
       <c r="D246" s="10">
         <v>245</v>
       </c>
-      <c r="E246" s="26"/>
-      <c r="F246" s="23"/>
-      <c r="G246" s="26"/>
+      <c r="E246" s="23"/>
+      <c r="F246" s="20"/>
+      <c r="G246" s="23"/>
       <c r="H246"/>
     </row>
     <row r="247" spans="2:8" x14ac:dyDescent="0.2">
@@ -3682,9 +3679,9 @@
       <c r="D247" s="5">
         <v>246</v>
       </c>
-      <c r="E247" s="26"/>
-      <c r="F247" s="23"/>
-      <c r="G247" s="26"/>
+      <c r="E247" s="23"/>
+      <c r="F247" s="20"/>
+      <c r="G247" s="23"/>
       <c r="H247"/>
     </row>
     <row r="248" spans="2:8" x14ac:dyDescent="0.2">
@@ -3694,9 +3691,9 @@
       <c r="D248" s="10">
         <v>247</v>
       </c>
-      <c r="E248" s="26"/>
-      <c r="F248" s="23"/>
-      <c r="G248" s="26"/>
+      <c r="E248" s="23"/>
+      <c r="F248" s="20"/>
+      <c r="G248" s="23"/>
       <c r="H248"/>
     </row>
     <row r="249" spans="2:8" x14ac:dyDescent="0.2">
@@ -3706,9 +3703,9 @@
       <c r="D249" s="5">
         <v>248</v>
       </c>
-      <c r="E249" s="26"/>
-      <c r="F249" s="23"/>
-      <c r="G249" s="26"/>
+      <c r="E249" s="23"/>
+      <c r="F249" s="20"/>
+      <c r="G249" s="23"/>
       <c r="H249"/>
     </row>
     <row r="250" spans="2:8" x14ac:dyDescent="0.2">
@@ -3718,9 +3715,9 @@
       <c r="D250" s="10">
         <v>249</v>
       </c>
-      <c r="E250" s="26"/>
-      <c r="F250" s="23"/>
-      <c r="G250" s="26"/>
+      <c r="E250" s="23"/>
+      <c r="F250" s="20"/>
+      <c r="G250" s="23"/>
       <c r="H250"/>
     </row>
     <row r="251" spans="2:8" x14ac:dyDescent="0.2">
@@ -3730,9 +3727,9 @@
       <c r="D251" s="5">
         <v>250</v>
       </c>
-      <c r="E251" s="26"/>
-      <c r="F251" s="23"/>
-      <c r="G251" s="26"/>
+      <c r="E251" s="23"/>
+      <c r="F251" s="20"/>
+      <c r="G251" s="23"/>
       <c r="H251"/>
     </row>
     <row r="252" spans="2:8" x14ac:dyDescent="0.2">
@@ -3742,9 +3739,9 @@
       <c r="D252" s="10">
         <v>251</v>
       </c>
-      <c r="E252" s="26"/>
-      <c r="F252" s="23"/>
-      <c r="G252" s="26"/>
+      <c r="E252" s="23"/>
+      <c r="F252" s="20"/>
+      <c r="G252" s="23"/>
       <c r="H252"/>
     </row>
     <row r="253" spans="2:8" x14ac:dyDescent="0.2">
@@ -3754,22 +3751,22 @@
       <c r="D253" s="5">
         <v>252</v>
       </c>
-      <c r="E253" s="26"/>
-      <c r="F253" s="23"/>
-      <c r="G253" s="26"/>
+      <c r="E253" s="23"/>
+      <c r="F253" s="20"/>
+      <c r="G253" s="23"/>
       <c r="H253"/>
     </row>
     <row r="254" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B254" s="21"/>
+      <c r="B254" s="18"/>
       <c r="C254" s="10">
         <v>253</v>
       </c>
       <c r="D254" s="10">
         <v>253</v>
       </c>
-      <c r="E254" s="26"/>
-      <c r="F254" s="23"/>
-      <c r="G254" s="26"/>
+      <c r="E254" s="23"/>
+      <c r="F254" s="20"/>
+      <c r="G254" s="23"/>
       <c r="H254"/>
     </row>
     <row r="255" spans="2:8" x14ac:dyDescent="0.2">
@@ -3780,36 +3777,36 @@
       <c r="D255" s="5">
         <v>254</v>
       </c>
-      <c r="E255" s="26"/>
-      <c r="F255" s="23"/>
-      <c r="G255" s="26"/>
+      <c r="E255" s="23"/>
+      <c r="F255" s="20"/>
+      <c r="G255" s="23"/>
       <c r="H255"/>
     </row>
     <row r="256" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B256" s="18"/>
+      <c r="B256" s="15"/>
       <c r="C256" s="10">
         <v>255</v>
       </c>
       <c r="D256" s="10">
         <v>255</v>
       </c>
-      <c r="E256" s="26"/>
-      <c r="F256" s="23"/>
-      <c r="G256" s="26"/>
+      <c r="E256" s="23"/>
+      <c r="F256" s="20"/>
+      <c r="G256" s="23"/>
       <c r="H256"/>
     </row>
     <row r="257" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B257" s="19"/>
+      <c r="B257" s="16"/>
       <c r="C257" s="12">
         <v>256</v>
       </c>
       <c r="D257" s="12">
         <v>256</v>
       </c>
-      <c r="E257" s="26"/>
-      <c r="F257" s="23"/>
-      <c r="G257" s="26"/>
-      <c r="H257" s="26"/>
+      <c r="E257" s="23"/>
+      <c r="F257" s="20"/>
+      <c r="G257" s="23"/>
+      <c r="H257" s="23"/>
     </row>
     <row r="258" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A258" s="8"/>

</xml_diff>